<commit_message>
Updated Tests (added test data in excel sheets)/commented login & home page/Added inspectors edit Id
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/EngineeringOfficesData.xlsx
+++ b/src/main/resources/testdata/EngineeringOfficesData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\MOMRA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\momra-e2e-tests\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1734D3B8-F711-418E-AEBA-BB358EB5243D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CAB154-F7F6-4F79-906D-65639FD64A8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BF483303-612B-4D37-B2F2-EEA758B6E25E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -67,6 +67,24 @@
   </si>
   <si>
     <t>ValidateOnTableLabelsAndColumnsOrder</t>
+  </si>
+  <si>
+    <t>إسم المكتب الهندسى</t>
+  </si>
+  <si>
+    <t>رقم المكتب الهندسى</t>
+  </si>
+  <si>
+    <t>الأمانة</t>
+  </si>
+  <si>
+    <t>البلدية</t>
+  </si>
+  <si>
+    <t>عدد المراقبين</t>
+  </si>
+  <si>
+    <t>الطاقة الإستيعابية (عدد الأسّرة)</t>
   </si>
 </sst>
 </file>
@@ -436,7 +454,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,10 +504,27 @@
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>